<commit_message>
added customer data to .xlsx
</commit_message>
<xml_diff>
--- a/src/python/comp-230/invoice_data.xlsx
+++ b/src/python/comp-230/invoice_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dalton/Code/cohort3/src/python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dalton/Code/cohort3/src/python/comp-230/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA3A5CB-BFF1-D248-904F-DA71B6A3FEDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFCAC602-DC11-5543-B733-D63F9DE91E9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="3" xr2:uid="{7E742BB3-A379-DC4A-8D47-23FDDF719C8F}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="line_items" sheetId="3" r:id="rId3"/>
     <sheet name="product_list" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="119">
   <si>
     <t>first_name</t>
   </si>
@@ -76,16 +78,358 @@
   </si>
   <si>
     <t>invoice_id</t>
+  </si>
+  <si>
+    <t>Leanne</t>
+  </si>
+  <si>
+    <t>Graham</t>
+  </si>
+  <si>
+    <t>Sincere@april.biz</t>
+  </si>
+  <si>
+    <t>45 Kulas Light, Apt. 556, Gwenborough</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>1-770-736-8031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ervin </t>
+  </si>
+  <si>
+    <t>Howell</t>
+  </si>
+  <si>
+    <t>Shanna@melissa.tv</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>35 Victor Plains, Suite 879, Wisokyburg</t>
+  </si>
+  <si>
+    <t>1-010-692-6599</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clementine </t>
+  </si>
+  <si>
+    <t>Bauch</t>
+  </si>
+  <si>
+    <t>Nathan@yesenia.net</t>
+  </si>
+  <si>
+    <t>1-463-123-4447</t>
+  </si>
+  <si>
+    <t>23 Douglas Extension, Suite 847, McKenziehaven</t>
+  </si>
+  <si>
+    <t>Patricia</t>
+  </si>
+  <si>
+    <t>Lebsack</t>
+  </si>
+  <si>
+    <t>Julianne.Oconner@kory.com</t>
+  </si>
+  <si>
+    <t>1-493-170-9623</t>
+  </si>
+  <si>
+    <t>68 Hoeger Mall, Apt. 692, South Elvis</t>
+  </si>
+  <si>
+    <t>Chelsey</t>
+  </si>
+  <si>
+    <t>Dietrich</t>
+  </si>
+  <si>
+    <t>Lucio_Hettinger@annie.ca</t>
+  </si>
+  <si>
+    <t>1-254-954-1289</t>
+  </si>
+  <si>
+    <t>75 Skiles Walks, Suite 351, Roscoeview</t>
+  </si>
+  <si>
+    <t>Dennis</t>
+  </si>
+  <si>
+    <t>Schulist</t>
+  </si>
+  <si>
+    <t>Karley_Dach@jasper.info</t>
+  </si>
+  <si>
+    <t>1 -477-935-8478</t>
+  </si>
+  <si>
+    <t>234 Norberto Crossing, Apt. 951, South Christy</t>
+  </si>
+  <si>
+    <t>Kurtis</t>
+  </si>
+  <si>
+    <t>Weissnat</t>
+  </si>
+  <si>
+    <t>Telly.Hoeger@billy.biz</t>
+  </si>
+  <si>
+    <t>1-210-067-6132</t>
+  </si>
+  <si>
+    <t>39 Rex Trail, Suite 280, Howemouth</t>
+  </si>
+  <si>
+    <t>Nicholas</t>
+  </si>
+  <si>
+    <t>Runolfsdottir</t>
+  </si>
+  <si>
+    <t>Sherwood@rosamond.me</t>
+  </si>
+  <si>
+    <t>1-586-493-6943</t>
+  </si>
+  <si>
+    <t>4826 Ellsworth Summit, Suite 279, Aliyaview</t>
+  </si>
+  <si>
+    <t>Glenna</t>
+  </si>
+  <si>
+    <t>Reichert</t>
+  </si>
+  <si>
+    <t>Chaim_McDermott@dana.io</t>
+  </si>
+  <si>
+    <t>1-755-976-6794</t>
+  </si>
+  <si>
+    <t>26 Dayna Park, Suite 449, Bartholomebury</t>
+  </si>
+  <si>
+    <t>Clementina</t>
+  </si>
+  <si>
+    <t>DuBuque</t>
+  </si>
+  <si>
+    <t>Ray.Padme@karina.com</t>
+  </si>
+  <si>
+    <t>1-024-648-3804</t>
+  </si>
+  <si>
+    <t>906 Kattie Turnpike, Suite 198, Lebsackbury</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>Payment for goods and services</t>
+  </si>
+  <si>
+    <t>shipping address</t>
+  </si>
+  <si>
+    <t>unit_price</t>
+  </si>
+  <si>
+    <t>301</t>
+  </si>
+  <si>
+    <t>302</t>
+  </si>
+  <si>
+    <t>303</t>
+  </si>
+  <si>
+    <t>304</t>
+  </si>
+  <si>
+    <t>305</t>
+  </si>
+  <si>
+    <t>306</t>
+  </si>
+  <si>
+    <t>307</t>
+  </si>
+  <si>
+    <t>308</t>
+  </si>
+  <si>
+    <t>309</t>
+  </si>
+  <si>
+    <t>310</t>
+  </si>
+  <si>
+    <t>Turbine</t>
+  </si>
+  <si>
+    <t>Pump</t>
+  </si>
+  <si>
+    <t>Heater</t>
+  </si>
+  <si>
+    <t>Blower</t>
+  </si>
+  <si>
+    <t>Tubing</t>
+  </si>
+  <si>
+    <t>prod_unit</t>
+  </si>
+  <si>
+    <t>pc.</t>
+  </si>
+  <si>
+    <t>Monitor</t>
+  </si>
+  <si>
+    <t>Markers</t>
+  </si>
+  <si>
+    <t>Board</t>
+  </si>
+  <si>
+    <t>Bucket</t>
+  </si>
+  <si>
+    <t>Desk</t>
+  </si>
+  <si>
+    <t>turbo turbine</t>
+  </si>
+  <si>
+    <t>jet pump</t>
+  </si>
+  <si>
+    <t>turbo heater</t>
+  </si>
+  <si>
+    <t>wonder blower</t>
+  </si>
+  <si>
+    <t>super tubing</t>
+  </si>
+  <si>
+    <t>power monitor</t>
+  </si>
+  <si>
+    <t>spring board</t>
+  </si>
+  <si>
+    <t>water markers</t>
+  </si>
+  <si>
+    <t>drain bucket</t>
+  </si>
+  <si>
+    <t>work desk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -108,13 +452,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -427,15 +782,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25B986DB-BB36-B84D-86D1-A6D28B854D7C}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F2" sqref="F2:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -451,27 +812,304 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="10:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="10:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="10:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="10:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="10:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="10:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="10:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="10:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="10:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="10:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="J26" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{0A36C5CC-E684-5C4C-B044-59B140E71FE9}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{24F74D6D-CBB4-7E4C-97C1-AF32A78AA98E}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{FAE040C5-D091-1D43-A0FE-F2292B957EB1}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{1B976D1D-E71D-9445-A00A-8A3082B084E7}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{DC974668-7F1F-2A40-B5C2-9FDB1AE820FE}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{0516D278-909F-B845-829F-6176DA7D7694}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{EE9972EF-90C8-1943-AC96-55FF74AF1C52}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{F829C9A3-747F-4242-B770-C24D561A9040}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{43696BC5-FE20-7E4F-B0DC-60AB87A064F2}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{3DBE3FFE-730D-F94F-A573-883CFA47C4FF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A2:A11" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04174DA-B418-B54F-B1E7-9F87AC115D23}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B1" t="s">
@@ -483,49 +1121,486 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="7">
+        <f ca="1">RANDBETWEEN(100,990)</f>
+        <v>397</v>
+      </c>
+      <c r="D2" s="6">
+        <f ca="1">RANDBETWEEN(DATE(2016,1,1),DATE(2016,12,31))</f>
+        <v>42421</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="7">
+        <f t="shared" ref="C3:C11" ca="1" si="0">RANDBETWEEN(100,990)</f>
+        <v>927</v>
+      </c>
+      <c r="D3" s="6">
+        <f t="shared" ref="D3:D11" ca="1" si="1">RANDBETWEEN(DATE(2016,1,1),DATE(2016,12,31))</f>
+        <v>42637</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>440</v>
+      </c>
+      <c r="D4" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>42716</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>856</v>
+      </c>
+      <c r="D5" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>42651</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>878</v>
+      </c>
+      <c r="D6" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>42701</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>793</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>42380</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>827</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>42492</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>119</v>
+      </c>
+      <c r="D9" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>42580</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>179</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>42386</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>352</v>
+      </c>
+      <c r="D11" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>42726</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E2:E11 A3:A11" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{362C9F12-1435-1B41-B9C0-226C20D5000B}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>201</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="5">
+        <v>101</v>
+      </c>
+      <c r="D2" s="7">
+        <f ca="1">RANDBETWEEN(1,20)</f>
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>202</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D11" ca="1" si="0">RANDBETWEEN(1,20)</f>
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E11" ca="1" si="1">RANDBETWEEN(1, 10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>203</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>12</v>
+      <c r="E4">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>204</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>205</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>206</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>207</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>208</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>209</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>210</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C3:C11 B2:B6 B7:B11" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB8205A0-83D2-424D-8D3F-F974D2D2C40A}">
-  <dimension ref="A2:C2"/>
+  <dimension ref="A2:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -535,8 +1610,155 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
+      <c r="D2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" t="s">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A3:A7 A8:A12" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor changes to id column
</commit_message>
<xml_diff>
--- a/src/python/comp-230/invoice_data.xlsx
+++ b/src/python/comp-230/invoice_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dalton/Code/cohort3/src/python/comp-230/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8082B6F0-F9B7-0A42-8DC1-B07EA712FBE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA89B2F-9189-D544-95EB-82EE4BC35D72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{7E742BB3-A379-DC4A-8D47-23FDDF719C8F}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="3" xr2:uid="{7E742BB3-A379-DC4A-8D47-23FDDF719C8F}"/>
   </bookViews>
   <sheets>
     <sheet name="customers" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>line_id</t>
-  </si>
-  <si>
     <t>cust_id</t>
   </si>
   <si>
@@ -393,6 +390,9 @@
   </si>
   <si>
     <t>work desk</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -784,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25B986DB-BB36-B84D-86D1-A6D28B854D7C}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -798,7 +798,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -813,217 +813,217 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
         <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
       </c>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" t="s">
         <v>37</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
       </c>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
         <v>40</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" t="s">
         <v>42</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>43</v>
-      </c>
-      <c r="F5" t="s">
-        <v>44</v>
       </c>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" t="s">
         <v>47</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>48</v>
-      </c>
-      <c r="F6" t="s">
-        <v>49</v>
       </c>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
         <v>50</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" t="s">
         <v>52</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>53</v>
-      </c>
-      <c r="F7" t="s">
-        <v>54</v>
       </c>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
         <v>55</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" t="s">
         <v>57</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>58</v>
-      </c>
-      <c r="F8" t="s">
-        <v>59</v>
       </c>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s">
         <v>60</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" t="s">
         <v>62</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>63</v>
-      </c>
-      <c r="F9" t="s">
-        <v>64</v>
       </c>
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
         <v>65</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" t="s">
         <v>67</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>68</v>
-      </c>
-      <c r="F10" t="s">
-        <v>69</v>
       </c>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
         <v>70</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" t="s">
         <v>72</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>73</v>
-      </c>
-      <c r="F11" t="s">
-        <v>74</v>
       </c>
       <c r="J11" s="2"/>
     </row>
@@ -1097,7 +1097,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1110,7 +1110,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -1122,10 +1122,10 @@
         <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1133,219 +1133,219 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="7">
         <f ca="1">RANDBETWEEN(100,990)</f>
-        <v>853</v>
+        <v>186</v>
       </c>
       <c r="D2" s="6">
         <f ca="1">RANDBETWEEN(DATE(2016,1,1),DATE(2016,12,31))</f>
-        <v>42461</v>
+        <v>42682</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" s="7">
         <f t="shared" ref="C3:C11" ca="1" si="0">RANDBETWEEN(100,990)</f>
-        <v>913</v>
+        <v>317</v>
       </c>
       <c r="D3" s="6">
         <f t="shared" ref="D3:D11" ca="1" si="1">RANDBETWEEN(DATE(2016,1,1),DATE(2016,12,31))</f>
-        <v>42603</v>
+        <v>42542</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>645</v>
+        <v>897</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>42678</v>
+        <v>42414</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>359</v>
+        <v>765</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>42495</v>
+        <v>42726</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>357</v>
+        <v>487</v>
       </c>
       <c r="D6" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>42672</v>
+        <v>42379</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C7" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>639</v>
+        <v>659</v>
       </c>
       <c r="D7" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>42587</v>
+        <v>42715</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>188</v>
+        <v>740</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>42529</v>
+        <v>42512</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>600</v>
+        <v>935</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>42519</v>
+        <v>42477</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>429</v>
+        <v>332</v>
       </c>
       <c r="D10" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>42533</v>
+        <v>42655</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s">
         <v>83</v>
-      </c>
-      <c r="B11" t="s">
-        <v>84</v>
       </c>
       <c r="C11" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>128</v>
+        <v>679</v>
       </c>
       <c r="D11" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>42656</v>
+        <v>42430</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1362,7 +1362,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1372,19 +1372,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1392,7 +1392,7 @@
         <v>201</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C2" s="5">
         <v>101</v>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(1, 10)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1411,10 +1411,10 @@
         <v>202</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" s="7">
         <f t="shared" ref="D3:D11" ca="1" si="0">RANDBETWEEN(1,20)</f>
@@ -1422,7 +1422,7 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E11" ca="1" si="1">RANDBETWEEN(1, 10)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1430,10 +1430,10 @@
         <v>203</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4" s="7">
         <f t="shared" ca="1" si="0"/>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1449,18 +1449,18 @@
         <v>204</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1468,14 +1468,14 @@
         <v>205</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
@@ -1487,18 +1487,18 @@
         <v>206</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D7" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1506,18 +1506,18 @@
         <v>207</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1525,18 +1525,18 @@
         <v>208</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1544,18 +1544,18 @@
         <v>209</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1563,18 +1563,18 @@
         <v>210</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D11" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1590,9 +1590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB8205A0-83D2-424D-8D3F-F974D2D2C40A}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1602,156 +1600,156 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>